<commit_message>
Commentaire et netoyage du code
</commit_message>
<xml_diff>
--- a/matrice d'implication.xlsx
+++ b/matrice d'implication.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79311E93-2D8D-4B31-A43F-17F7BD55934D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54479C51-3F6E-4301-8AB5-36CE2C445A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -802,20 +813,20 @@
   <dimension ref="B1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="9.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" style="1" customWidth="1"/>
     <col min="4" max="8" width="19" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="23" t="s">
         <v>6</v>
       </c>
@@ -826,7 +837,7 @@
       <c r="G2" s="24"/>
       <c r="H2" s="25"/>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="26"/>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
@@ -835,7 +846,7 @@
       <c r="G3" s="27"/>
       <c r="H3" s="28"/>
     </row>
-    <row r="4" spans="2:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
@@ -852,7 +863,7 @@
       </c>
       <c r="H4" s="33"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="29" t="s">
         <v>1</v>
       </c>
@@ -865,7 +876,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -882,7 +893,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
@@ -899,7 +910,7 @@
       <c r="G7" s="18"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <f>1+B7</f>
         <v>2</v>
@@ -908,16 +919,16 @@
         <v>15</v>
       </c>
       <c r="D8" s="21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <f t="shared" ref="B9:B34" si="0">1+B8</f>
         <v>3</v>
@@ -926,16 +937,16 @@
         <v>13</v>
       </c>
       <c r="D9" s="21">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E9" s="22">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -944,16 +955,16 @@
         <v>14</v>
       </c>
       <c r="D10" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="E10" s="22">
         <v>0.2</v>
-      </c>
-      <c r="E10" s="22">
-        <v>0.7</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -971,7 +982,7 @@
       <c r="G11" s="18"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -989,7 +1000,7 @@
       <c r="G12" s="18"/>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1001,7 +1012,7 @@
       <c r="G13" s="18"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1013,7 +1024,7 @@
       <c r="G14" s="18"/>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1025,7 +1036,7 @@
       <c r="G15" s="18"/>
       <c r="H15" s="20"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1037,7 +1048,7 @@
       <c r="G16" s="18"/>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1049,7 +1060,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="20"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1061,7 +1072,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="20"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1073,7 +1084,7 @@
       <c r="G19" s="18"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1085,7 +1096,7 @@
       <c r="G20" s="18"/>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1097,7 +1108,7 @@
       <c r="G21" s="18"/>
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1109,7 +1120,7 @@
       <c r="G22" s="18"/>
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1121,7 +1132,7 @@
       <c r="G23" s="18"/>
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1133,7 +1144,7 @@
       <c r="G24" s="18"/>
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1145,7 +1156,7 @@
       <c r="G25" s="18"/>
       <c r="H25" s="20"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1157,7 +1168,7 @@
       <c r="G26" s="18"/>
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1169,7 +1180,7 @@
       <c r="G27" s="18"/>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1181,7 +1192,7 @@
       <c r="G28" s="18"/>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1193,7 +1204,7 @@
       <c r="G29" s="18"/>
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1205,7 +1216,7 @@
       <c r="G30" s="18"/>
       <c r="H30" s="20"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1217,7 +1228,7 @@
       <c r="G31" s="18"/>
       <c r="H31" s="20"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1229,7 +1240,7 @@
       <c r="G32" s="18"/>
       <c r="H32" s="20"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1241,7 +1252,7 @@
       <c r="G33" s="18"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1253,7 +1264,7 @@
       <c r="G34" s="18"/>
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
       <c r="C35" s="7"/>
       <c r="D35" s="9"/>
@@ -1262,7 +1273,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="17" t="s">
         <v>5</v>
       </c>
@@ -1273,27 +1284,27 @@
       <c r="G36" s="12"/>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="14"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="14"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" s="14"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" s="14"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" s="14"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="15"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16"/>

</xml_diff>